<commit_message>
new book version and structure
</commit_message>
<xml_diff>
--- a/data/flea_dog_cat_foxes.xlsx
+++ b/data/flea_dog_cat_foxes.xlsx
@@ -412,7 +412,7 @@
         <v>22</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -429,7 +429,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -446,7 +446,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -514,7 +514,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -565,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>

</xml_diff>